<commit_message>
Committing QGIS file, plus final README update
</commit_message>
<xml_diff>
--- a/data/results/Wildfire_risk_analysis_results.xlsx
+++ b/data/results/Wildfire_risk_analysis_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesrco/Code/DeCoLandUse/data/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23ACAC4D-3860-1E44-8019-65EDCDB4D94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC7D2D4-F76A-8A44-8C4E-B598CD5C31FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{4B44BC70-DFED-A445-9A97-5138A0186887}"/>
   </bookViews>
@@ -544,7 +544,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>